<commit_message>
add template tag for fraud type for police letter
</commit_message>
<xml_diff>
--- a/Input Data/Police Letter Template/Case 2/PoliceLetter V2 Case 28 Intelligence 2.xlsx
+++ b/Input Data/Police Letter Template/Case 2/PoliceLetter V2 Case 28 Intelligence 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\hase-scripts\Input Data\Police Letter Template\Case 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38FEAF5-1943-48EC-BB16-304AE1CB320B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ECC7070-FF5A-4172-BDAB-FF81482A5A84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="6690" windowWidth="29040" windowHeight="15720" tabRatio="859" activeTab="4" xr2:uid="{87512554-1306-F949-B1A5-DEDDB9062EFE}"/>
   </bookViews>
@@ -1264,8 +1264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F12BFACA-6A18-5247-8684-55BDA2AEE25C}">
   <dimension ref="B1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1337,6 +1337,7 @@
       <c r="B6" s="2" t="str">
         <f>_xlfn.LET(
   _xlpm.rows_3,
+    "&lt;Template_FraudTypeCheckbox&gt;" &amp;
     "&lt;tr&gt;&lt;th colspan='3'&gt;" &amp; 'PoliceLetter-Template'!B26 &amp; "&lt;/th&gt;&lt;tr&gt;" &amp;
     "&lt;tr&gt;&lt;td colspan='3'&gt; - [" &amp; IF('PoliceLetter-TypeOfDeception'!A2 = "Y", "X", " ") &amp; "] " &amp; 'PoliceLetter-Template'!B27 &amp; "&lt;/td&gt;&lt;/tr&gt;" &amp;
     "&lt;tr&gt;&lt;td colspan='3'&gt; - [" &amp; IF('PoliceLetter-TypeOfDeception'!B2 = "Y", "X", " ") &amp; "] " &amp; 'PoliceLetter-Template'!B28 &amp; "&lt;/td&gt;&lt;/tr&gt;" &amp;
@@ -1344,10 +1345,11 @@
     "&lt;tr&gt;&lt;td colspan='3'&gt; - [" &amp; IF('PoliceLetter-TypeOfDeception'!D2 = "Y", "X", " ") &amp; "] " &amp; 'PoliceLetter-Template'!B30 &amp; "&lt;/td&gt;&lt;/tr&gt;" &amp;
     "&lt;tr&gt;&lt;td colspan='3'&gt; - [" &amp; IF('PoliceLetter-TypeOfDeception'!E2 = "Y", "X", " ") &amp; "] " &amp; 'PoliceLetter-Template'!B31 &amp; "&lt;/td&gt;&lt;/tr&gt;" &amp;
     "&lt;tr&gt;&lt;td colspan='3'&gt; - [" &amp; IF('PoliceLetter-TypeOfDeception'!F2 &lt;&gt; "", "X", " ") &amp; "] " &amp; 'PoliceLetter-Template'!B25 &amp; " " &amp; 'PoliceLetter-TypeOfDeception'!F2 &amp; "&lt;/td&gt;&lt;/tr&gt;" &amp;
-    "&lt;tr&gt;&lt;td colspan='3'&gt;" &amp; 'PoliceLetter-Template'!B32 &amp; "&lt;/td&gt;&lt;/tr&gt;",
+    "&lt;tr&gt;&lt;td colspan='3'&gt;" &amp; 'PoliceLetter-Template'!B32 &amp; "&lt;/td&gt;&lt;/tr&gt;" &amp;
+    "&lt;/Template_FraudTypeCheckbox&gt;",
   _xlpm.rows_3
 )</f>
-        <v>&lt;tr&gt;&lt;th colspan='3'&gt;If the predicate offence is deception related, please state the type of deception:&lt;/th&gt;&lt;tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Telephone Deception&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] E-shopping Fraud&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Romance Scam&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [X] Investment Scam&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Employment Fraud&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Others (please specify) &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt;(please tick if appropriate)&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;Template_FraudTypeCheckbox&gt;&lt;tr&gt;&lt;th colspan='3'&gt;If the predicate offence is deception related, please state the type of deception:&lt;/th&gt;&lt;tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Telephone Deception&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] E-shopping Fraud&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Romance Scam&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [X] Investment Scam&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Employment Fraud&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Others (please specify) &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt;(please tick if appropriate)&lt;/td&gt;&lt;/tr&gt;&lt;/Template_FraudTypeCheckbox&gt;</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="138.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -1438,7 +1440,7 @@
 &lt;tbody&gt;
 &lt;tr&gt;&lt;th&gt;Account Name:&lt;/th&gt;&lt;td colspan='2'&gt;&lt;Template_Suspect2_Name&gt;CHUNG SIU &lt;/Template_Suspect2_Name&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th&gt;Account Number:&lt;/th&gt;&lt;td colspan='2'&gt;&lt;Template_Suspect2_AccountNumber&gt;111-111111-102 &lt;/Template_Suspect2_AccountNumber&gt;&lt;/td&gt;&lt;/tr&gt;
 &lt;tr&gt;&lt;th colspan='3'&gt;Suspected nature of transactions:&lt;/th&gt;&lt;tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [X] Might have been used in receicing proceeds of crime&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Might have been used to receive funds related to terrorist financing&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Exhibited transaction patterns which were incommensurate with holder's background&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Others (please specify) &lt;/td&gt;&lt;/tr&gt;
-&lt;tr&gt;&lt;th colspan='3'&gt;If the predicate offence is deception related, please state the type of deception:&lt;/th&gt;&lt;tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Telephone Deception&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] E-shopping Fraud&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Romance Scam&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [X] Investment Scam&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Employment Fraud&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Others (please specify) &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt;(please tick if appropriate)&lt;/td&gt;&lt;/tr&gt;
+&lt;Template_FraudTypeCheckbox&gt;&lt;tr&gt;&lt;th colspan='3'&gt;If the predicate offence is deception related, please state the type of deception:&lt;/th&gt;&lt;tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Telephone Deception&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] E-shopping Fraud&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Romance Scam&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [X] Investment Scam&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Employment Fraud&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Others (please specify) &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt;(please tick if appropriate)&lt;/td&gt;&lt;/tr&gt;&lt;/Template_FraudTypeCheckbox&gt;
 &lt;tr&gt;&lt;th colspan='3'&gt;Transaction Details:&lt;/th&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th&gt;Date&lt;/th&gt;&lt;th&gt;Amount&lt;/th&gt;&lt;th&gt;Transferor's Bank and Account&lt;/th&gt;&lt;/tr&gt;
 &lt;tr&gt;&lt;td&gt;&lt;Template_Located_FraudPayment3_Date&gt;2024-08-28&lt;/Template_Located_FraudPayment3_Date&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Located_FraudPayment3_Amount&gt;50000&lt;/Template_Located_FraudPayment3_Amount&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Victim0_Account0_Bank&gt;NA&lt;/Template_Victim0_Account0_Bank&gt; &lt;Template_Victim0_Account0_AccountNumber&gt;Cash&lt;/Template_Victim0_Account0_AccountNumber&gt;&lt;/td&gt;&lt;/tr&gt;
 &lt;tr&gt;&lt;th colspan='3'&gt;Case Summary:&lt;/th&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt;On 2024-08-22, a female reported to police that on 2024-09-09, she was lured to invest into
@@ -1850,7 +1852,7 @@
 &lt;tbody&gt;
 &lt;tr&gt;&lt;th&gt;Account Name:&lt;/th&gt;&lt;td colspan='2'&gt;&lt;Template_Suspect2_Name&gt;CHUNG SIU &lt;/Template_Suspect2_Name&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th&gt;Account Number:&lt;/th&gt;&lt;td colspan='2'&gt;&lt;Template_Suspect2_AccountNumber&gt;111-111111-102 &lt;/Template_Suspect2_AccountNumber&gt;&lt;/td&gt;&lt;/tr&gt;
 &lt;tr&gt;&lt;th colspan='3'&gt;Suspected nature of transactions:&lt;/th&gt;&lt;tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [X] Might have been used in receicing proceeds of crime&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Might have been used to receive funds related to terrorist financing&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Exhibited transaction patterns which were incommensurate with holder's background&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Others (please specify) &lt;/td&gt;&lt;/tr&gt;
-&lt;tr&gt;&lt;th colspan='3'&gt;If the predicate offence is deception related, please state the type of deception:&lt;/th&gt;&lt;tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Telephone Deception&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] E-shopping Fraud&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Romance Scam&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [X] Investment Scam&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Employment Fraud&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Others (please specify) &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt;(please tick if appropriate)&lt;/td&gt;&lt;/tr&gt;
+&lt;Template_FraudTypeCheckbox&gt;&lt;tr&gt;&lt;th colspan='3'&gt;If the predicate offence is deception related, please state the type of deception:&lt;/th&gt;&lt;tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Telephone Deception&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] E-shopping Fraud&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Romance Scam&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [X] Investment Scam&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Employment Fraud&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Others (please specify) &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt;(please tick if appropriate)&lt;/td&gt;&lt;/tr&gt;&lt;/Template_FraudTypeCheckbox&gt;
 &lt;tr&gt;&lt;th colspan='3'&gt;Transaction Details:&lt;/th&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th&gt;Date&lt;/th&gt;&lt;th&gt;Amount&lt;/th&gt;&lt;th&gt;Transferor's Bank and Account&lt;/th&gt;&lt;/tr&gt;
 &lt;tr&gt;&lt;td&gt;&lt;Template_Located_FraudPayment3_Date&gt;2024-08-28&lt;/Template_Located_FraudPayment3_Date&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Located_FraudPayment3_Amount&gt;50000&lt;/Template_Located_FraudPayment3_Amount&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Victim0_Account0_Bank&gt;NA&lt;/Template_Victim0_Account0_Bank&gt; &lt;Template_Victim0_Account0_AccountNumber&gt;Cash&lt;/Template_Victim0_Account0_AccountNumber&gt;&lt;/td&gt;&lt;/tr&gt;
 &lt;tr&gt;&lt;th colspan='3'&gt;Case Summary:&lt;/th&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt;On 2024-08-22, a female reported to police that on 2024-09-09, she was lured to invest into

</xml_diff>